<commit_message>
var div update macro data
</commit_message>
<xml_diff>
--- a/FinancialPlanner/data/Macro_data_poland.xlsx
+++ b/FinancialPlanner/data/Macro_data_poland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja_portfela\FinancialPlanner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476D082D-4ACC-42DC-88DB-452CBECF4D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB29F14-F797-421E-9CA3-C3631074660C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>observation_date</t>
   </si>
@@ -65,19 +65,27 @@
   <si>
     <t>Data Updated: 2025-09-01</t>
   </si>
+  <si>
+    <t>NGDPSAXDCPLQ</t>
+  </si>
+  <si>
+    <t>POLCPIALLQINMEI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000000000000000"/>
     <numFmt numFmtId="167" formatCode="#,##0.00000000000000000"/>
     <numFmt numFmtId="168" formatCode="#,##0.0000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +106,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -137,11 +153,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +227,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +601,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:XFD99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,9 +614,11 @@
     <col min="3" max="3" width="23.109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.109375" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,8 +634,14 @@
       <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>36892</v>
       </c>
@@ -613,8 +657,14 @@
       <c r="E2" s="14">
         <v>76.894963343005898</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="21">
+        <v>193338.3</v>
+      </c>
+      <c r="G2" s="22">
+        <v>73.027969999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>36982</v>
       </c>
@@ -630,8 +680,14 @@
       <c r="E3" s="14">
         <v>78.293315496321895</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="21">
+        <v>196278.6</v>
+      </c>
+      <c r="G3" s="22">
+        <v>74.387720000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>37073</v>
       </c>
@@ -647,8 +703,14 @@
       <c r="E4" s="14">
         <v>78.545285977919207</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="21">
+        <v>197852.5</v>
+      </c>
+      <c r="G4" s="22">
+        <v>74.340830000000011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>37165</v>
       </c>
@@ -664,8 +726,14 @@
       <c r="E5" s="14">
         <v>78.975249992711895</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="21">
+        <v>198798.3</v>
+      </c>
+      <c r="G5" s="22">
+        <v>74.786270000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>37257</v>
       </c>
@@ -681,8 +749,14 @@
       <c r="E6" s="14">
         <v>80.017248929514196</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="21">
+        <v>202698.1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>75.630250000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>37347</v>
       </c>
@@ -698,8 +772,14 @@
       <c r="E7" s="14">
         <v>79.429304860526599</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="21">
+        <v>202548.3</v>
+      </c>
+      <c r="G7" s="22">
+        <v>75.911580000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>37438</v>
       </c>
@@ -715,8 +795,14 @@
       <c r="E8" s="14">
         <v>79.621953573021202</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="21">
+        <v>204974.3</v>
+      </c>
+      <c r="G8" s="22">
+        <v>75.208259999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>37530</v>
       </c>
@@ -732,8 +818,14 @@
       <c r="E9" s="14">
         <v>79.4131586815719</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="21">
+        <v>205468.3</v>
+      </c>
+      <c r="G9" s="22">
+        <v>75.442700000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>37622</v>
       </c>
@@ -749,8 +841,14 @@
       <c r="E10" s="14">
         <v>79.629065584477601</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="21">
+        <v>206897.9</v>
+      </c>
+      <c r="G10" s="22">
+        <v>75.864689999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>37712</v>
       </c>
@@ -766,8 +864,14 @@
       <c r="E11" s="14">
         <v>80.100909986599802</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="21">
+        <v>211594.4</v>
+      </c>
+      <c r="G11" s="22">
+        <v>76.146019999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>37803</v>
       </c>
@@ -783,8 +887,14 @@
       <c r="E12" s="14">
         <v>79.969451943917605</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="21">
+        <v>213973.1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>75.747469999999979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>37895</v>
       </c>
@@ -800,8 +910,14 @@
       <c r="E13" s="14">
         <v>80.715544931786994</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="21">
+        <v>217655.5</v>
+      </c>
+      <c r="G13" s="22">
+        <v>76.497669999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>37987</v>
       </c>
@@ -817,8 +933,14 @@
       <c r="E14" s="14">
         <v>82.192285697429995</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="21">
+        <v>226881</v>
+      </c>
+      <c r="G14" s="22">
+        <v>77.060330000000022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>38078</v>
       </c>
@@ -834,8 +956,14 @@
       <c r="E15" s="14">
         <v>82.891073452850307</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="21">
+        <v>230717.6</v>
+      </c>
+      <c r="G15" s="22">
+        <v>78.607640000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>38169</v>
       </c>
@@ -851,8 +979,14 @@
       <c r="E16" s="14">
         <v>84.588047863149498</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="21">
+        <v>235316</v>
+      </c>
+      <c r="G16" s="22">
+        <v>79.099959999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>38261</v>
       </c>
@@ -868,8 +1002,14 @@
       <c r="E17" s="14">
         <v>86.574735009837795</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="21">
+        <v>243195.5</v>
+      </c>
+      <c r="G17" s="22">
+        <v>79.779830000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>38353</v>
       </c>
@@ -885,8 +1025,14 @@
       <c r="E18" s="14">
         <v>85.980582425278001</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="21">
+        <v>242865.5</v>
+      </c>
+      <c r="G18" s="22">
+        <v>79.943939999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>38443</v>
       </c>
@@ -902,8 +1048,14 @@
       <c r="E19" s="14">
         <v>87.3444241199755</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="21">
+        <v>247860.7</v>
+      </c>
+      <c r="G19" s="22">
+        <v>80.412819999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>38534</v>
       </c>
@@ -919,8 +1071,14 @@
       <c r="E20" s="14">
         <v>86.827788587057597</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="21">
+        <v>250833.8</v>
+      </c>
+      <c r="G20" s="22">
+        <v>80.319050000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>38626</v>
       </c>
@@ -936,8 +1094,14 @@
       <c r="E21" s="14">
         <v>85.520963417532897</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="21">
+        <v>251502.8</v>
+      </c>
+      <c r="G21" s="22">
+        <v>80.741039999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>38718</v>
       </c>
@@ -953,8 +1117,14 @@
       <c r="E22" s="14">
         <v>86.440766065092802</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="21">
+        <v>258179.8</v>
+      </c>
+      <c r="G22" s="22">
+        <v>80.72175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>38808</v>
       </c>
@@ -970,8 +1140,14 @@
       <c r="E23" s="14">
         <v>86.162729325220297</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="21">
+        <v>263328.7</v>
+      </c>
+      <c r="G23" s="22">
+        <v>81.400080000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>38899</v>
       </c>
@@ -987,8 +1163,14 @@
       <c r="E24" s="14">
         <v>87.538163921991796</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="21">
+        <v>271894.8</v>
+      </c>
+      <c r="G24" s="22">
+        <v>81.671419999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>38991</v>
       </c>
@@ -1004,8 +1186,14 @@
       <c r="E25" s="14">
         <v>91.026099859842603</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="21">
+        <v>278825.7</v>
+      </c>
+      <c r="G25" s="22">
+        <v>81.75282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>39083</v>
       </c>
@@ -1021,8 +1209,14 @@
       <c r="E26" s="14">
         <v>89.673561050899195</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="21">
+        <v>286003.59999999998</v>
+      </c>
+      <c r="G26" s="22">
+        <v>82.34975</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>39173</v>
       </c>
@@ -1038,8 +1232,14 @@
       <c r="E27" s="14">
         <v>90.803950328087197</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="21">
+        <v>293392.90000000002</v>
+      </c>
+      <c r="G27" s="22">
+        <v>83.380809999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>39264</v>
       </c>
@@ -1055,8 +1255,14 @@
       <c r="E28" s="14">
         <v>91.069265793349402</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="21">
+        <v>299399.3</v>
+      </c>
+      <c r="G28" s="22">
+        <v>83.272289999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>39356</v>
       </c>
@@ -1072,8 +1278,14 @@
       <c r="E29" s="14">
         <v>92.887972061549803</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="21">
+        <v>309577.09999999998</v>
+      </c>
+      <c r="G29" s="22">
+        <v>84.547550000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>39448</v>
       </c>
@@ -1089,8 +1301,14 @@
       <c r="E30" s="14">
         <v>93.461726365320402</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="21">
+        <v>316425.7</v>
+      </c>
+      <c r="G30" s="22">
+        <v>85.795680000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>39539</v>
       </c>
@@ -1106,8 +1324,14 @@
       <c r="E31" s="14">
         <v>94.068272174033595</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="21">
+        <v>320226.09999999998</v>
+      </c>
+      <c r="G31" s="22">
+        <v>86.935290000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>39630</v>
       </c>
@@ -1123,8 +1347,14 @@
       <c r="E32" s="14">
         <v>95.281266869271505</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="21">
+        <v>324238</v>
+      </c>
+      <c r="G32" s="22">
+        <v>87.125219999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>39722</v>
       </c>
@@ -1140,8 +1370,14 @@
       <c r="E33" s="14">
         <v>96.390539294950798</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="21">
+        <v>328590.09999999998</v>
+      </c>
+      <c r="G33" s="22">
+        <v>87.586489999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>39814</v>
       </c>
@@ -1157,8 +1393,14 @@
       <c r="E34" s="14">
         <v>97.894791614120805</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="21">
+        <v>337663.5</v>
+      </c>
+      <c r="G34" s="22">
+        <v>88.753219999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>39904</v>
       </c>
@@ -1174,8 +1416,14 @@
       <c r="E35" s="14">
         <v>98.243812009378203</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="21">
+        <v>339638.3</v>
+      </c>
+      <c r="G35" s="22">
+        <v>90.489750000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>39995</v>
       </c>
@@ -1191,8 +1439,14 @@
       <c r="E36" s="14">
         <v>99.241540283812895</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="21">
+        <v>345709.5</v>
+      </c>
+      <c r="G36" s="22">
+        <v>90.625429999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>40087</v>
       </c>
@@ -1208,8 +1462,14 @@
       <c r="E37" s="14">
         <v>98.820303717634701</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="21">
+        <v>350144.4</v>
+      </c>
+      <c r="G37" s="22">
+        <v>90.761089999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>40179</v>
       </c>
@@ -1225,8 +1485,14 @@
       <c r="E38" s="14">
         <v>98.921676115229502</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F38" s="21">
+        <v>349237.2</v>
+      </c>
+      <c r="G38" s="22">
+        <v>91.602230000000006</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>40269</v>
       </c>
@@ -1242,8 +1508,14 @@
       <c r="E39" s="14">
         <v>99.928389301985007</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="21">
+        <v>358042.1</v>
+      </c>
+      <c r="G39" s="22">
+        <v>92.470489999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>40360</v>
       </c>
@@ -1259,8 +1531,14 @@
       <c r="E40" s="14">
         <v>100.315209807911</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="21">
+        <v>363652.2</v>
+      </c>
+      <c r="G40" s="22">
+        <v>92.470489999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40452</v>
       </c>
@@ -1276,8 +1554,14 @@
       <c r="E41" s="14">
         <v>100.834724774874</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F41" s="21">
+        <v>368568</v>
+      </c>
+      <c r="G41" s="22">
+        <v>93.393029999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>40544</v>
       </c>
@@ -1293,8 +1577,14 @@
       <c r="E42" s="14">
         <v>102.165618320842</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F42" s="21">
+        <v>380146.1</v>
+      </c>
+      <c r="G42" s="22">
+        <v>95.238100000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>40634</v>
       </c>
@@ -1310,8 +1600,14 @@
       <c r="E43" s="14">
         <v>102.41824040180001</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="21">
+        <v>385903.2</v>
+      </c>
+      <c r="G43" s="22">
+        <v>96.621889999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>40725</v>
       </c>
@@ -1327,8 +1623,14 @@
       <c r="E44" s="14">
         <v>103.146217160535</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="21">
+        <v>393193.1</v>
+      </c>
+      <c r="G44" s="22">
+        <v>96.24203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>40817</v>
       </c>
@@ -1344,8 +1646,14 @@
       <c r="E45" s="14">
         <v>104.414285679041</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F45" s="21">
+        <v>401717</v>
+      </c>
+      <c r="G45" s="22">
+        <v>97.517300000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>40909</v>
       </c>
@@ -1361,8 +1669,14 @@
       <c r="E46" s="14">
         <v>104.43708174846</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="21">
+        <v>402660.9</v>
+      </c>
+      <c r="G46" s="22">
+        <v>99.091030000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>41000</v>
       </c>
@@ -1378,8 +1692,14 @@
       <c r="E47" s="14">
         <v>105.59273883290101</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F47" s="21">
+        <v>406215</v>
+      </c>
+      <c r="G47" s="22">
+        <v>100.28489999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>41091</v>
       </c>
@@ -1395,8 +1715,14 @@
       <c r="E48" s="14">
         <v>105.85263346457999</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F48" s="21">
+        <v>407412.3</v>
+      </c>
+      <c r="G48" s="22">
+        <v>99.769360000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>41183</v>
       </c>
@@ -1412,8 +1738,14 @@
       <c r="E49" s="14">
         <v>105.305269379804</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="21">
+        <v>404878.6</v>
+      </c>
+      <c r="G49" s="22">
+        <v>100.20350000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>41275</v>
       </c>
@@ -1429,8 +1761,14 @@
       <c r="E50" s="14">
         <v>105.05631914588299</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="21">
+        <v>402813</v>
+      </c>
+      <c r="G50" s="22">
+        <v>100.42059999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>41365</v>
       </c>
@@ -1446,8 +1784,14 @@
       <c r="E51" s="14">
         <v>105.46713715710101</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="21">
+        <v>407447.1</v>
+      </c>
+      <c r="G51" s="22">
+        <v>100.8818</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>41456</v>
       </c>
@@ -1463,8 +1807,14 @@
       <c r="E52" s="14">
         <v>105.280180904201</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="21">
+        <v>409704.7</v>
+      </c>
+      <c r="G52" s="22">
+        <v>100.99039999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>41548</v>
       </c>
@@ -1480,8 +1830,14 @@
       <c r="E53" s="14">
         <v>106.66218578207101</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="21">
+        <v>417405.8</v>
+      </c>
+      <c r="G53" s="22">
+        <v>101.0175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>41640</v>
       </c>
@@ -1497,8 +1853,14 @@
       <c r="E54" s="14">
         <v>106.57146064627</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="21">
+        <v>422628.3</v>
+      </c>
+      <c r="G54" s="22">
+        <v>101.1803</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>41730</v>
       </c>
@@ -1514,8 +1876,14 @@
       <c r="E55" s="14">
         <v>106.11737090817201</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F55" s="21">
+        <v>425598.2</v>
+      </c>
+      <c r="G55" s="22">
+        <v>101.20740000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>41821</v>
       </c>
@@ -1531,8 +1899,14 @@
       <c r="E56" s="14">
         <v>106.74641544134499</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="21">
+        <v>431595.5</v>
+      </c>
+      <c r="G56" s="22">
+        <v>100.7462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>41913</v>
       </c>
@@ -1548,8 +1922,14 @@
       <c r="E57" s="14">
         <v>105.413389715378</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="21">
+        <v>429837.7</v>
+      </c>
+      <c r="G57" s="22">
+        <v>100.3934</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>42005</v>
       </c>
@@ -1565,8 +1945,14 @@
       <c r="E58" s="14">
         <v>106.571558994762</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="21">
+        <v>441667.7</v>
+      </c>
+      <c r="G58" s="22">
+        <v>99.959299999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>42095</v>
       </c>
@@ -1582,8 +1968,14 @@
       <c r="E59" s="14">
         <v>107.37176744742401</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F59" s="21">
+        <v>447523.1</v>
+      </c>
+      <c r="G59" s="22">
+        <v>100.4477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>42186</v>
       </c>
@@ -1599,8 +1991,14 @@
       <c r="E60" s="14">
         <v>107.251329852113</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F60" s="21">
+        <v>452999.4</v>
+      </c>
+      <c r="G60" s="22">
+        <v>99.986429999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>42278</v>
       </c>
@@ -1616,8 +2014,14 @@
       <c r="E61" s="14">
         <v>109.003360215898</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F61" s="21">
+        <v>464307.7</v>
+      </c>
+      <c r="G61" s="22">
+        <v>99.606570000000005</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>42370</v>
       </c>
@@ -1633,8 +2037,14 @@
       <c r="E62" s="14">
         <v>107.711955045631</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F62" s="21">
+        <v>457989.3</v>
+      </c>
+      <c r="G62" s="22">
+        <v>98.955370000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>42461</v>
       </c>
@@ -1650,8 +2060,14 @@
       <c r="E63" s="14">
         <v>107.63239711220599</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F63" s="21">
+        <v>464398.1</v>
+      </c>
+      <c r="G63" s="22">
+        <v>99.416629999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>42552</v>
       </c>
@@ -1667,8 +2083,14 @@
       <c r="E64" s="14">
         <v>107.747830661856</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F64" s="21">
+        <v>467605.7</v>
+      </c>
+      <c r="G64" s="22">
+        <v>99.118160000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>42644</v>
       </c>
@@ -1684,8 +2106,14 @@
       <c r="E65" s="14">
         <v>107.73318334792199</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="21">
+        <v>476585.8</v>
+      </c>
+      <c r="G65" s="22">
+        <v>99.850769999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>42736</v>
       </c>
@@ -1701,8 +2129,14 @@
       <c r="E66" s="14">
         <v>109.12565787153299</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F66" s="21">
+        <v>488395.6</v>
+      </c>
+      <c r="G66" s="22">
+        <v>100.9632</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>42826</v>
       </c>
@@ -1718,8 +2152,14 @@
       <c r="E67" s="14">
         <v>109.49913503721</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F67" s="21">
+        <v>494894.2</v>
+      </c>
+      <c r="G67" s="22">
+        <v>101.28879999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>42917</v>
       </c>
@@ -1735,8 +2175,14 @@
       <c r="E68" s="14">
         <v>109.654767047959</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F68" s="21">
+        <v>503030.5</v>
+      </c>
+      <c r="G68" s="22">
+        <v>101.0989</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>43009</v>
       </c>
@@ -1752,8 +2198,14 @@
       <c r="E69" s="14">
         <v>109.63922389967</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F69" s="21">
+        <v>510108.8</v>
+      </c>
+      <c r="G69" s="22">
+        <v>102.2385</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>43101</v>
       </c>
@@ -1769,8 +2221,14 @@
       <c r="E70" s="14">
         <v>110.005004012331</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F70" s="21">
+        <v>521952.3</v>
+      </c>
+      <c r="G70" s="22">
+        <v>102.6998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>43191</v>
       </c>
@@ -1786,8 +2244,14 @@
       <c r="E71" s="14">
         <v>110.10992520795899</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F71" s="21">
+        <v>530090.1</v>
+      </c>
+      <c r="G71" s="22">
+        <v>103.2424</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>43282</v>
       </c>
@@ -1803,8 +2267,14 @@
       <c r="E72" s="14">
         <v>110.976724157053</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F72" s="21">
+        <v>541015.6</v>
+      </c>
+      <c r="G72" s="22">
+        <v>103.2153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>43374</v>
       </c>
@@ -1820,8 +2290,14 @@
       <c r="E73" s="14">
         <v>112.26529524861201</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F73" s="21">
+        <v>552643.4</v>
+      </c>
+      <c r="G73" s="22">
+        <v>103.7851</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>43466</v>
       </c>
@@ -1837,8 +2313,14 @@
       <c r="E74" s="14">
         <v>112.788320410754</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F74" s="21">
+        <v>563275.9</v>
+      </c>
+      <c r="G74" s="22">
+        <v>103.9208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>43556</v>
       </c>
@@ -1854,8 +2336,14 @@
       <c r="E75" s="14">
         <v>114.439270381434</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F75" s="21">
+        <v>576832.80000000005</v>
+      </c>
+      <c r="G75" s="22">
+        <v>105.6844</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>43647</v>
       </c>
@@ -1871,8 +2359,14 @@
       <c r="E76" s="14">
         <v>113.94079432439401</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F76" s="21">
+        <v>578837.69999999995</v>
+      </c>
+      <c r="G76" s="22">
+        <v>105.9829</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>43739</v>
       </c>
@@ -1888,8 +2382,14 @@
       <c r="E77" s="14">
         <v>115.78179127703299</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F77" s="21">
+        <v>592387.4</v>
+      </c>
+      <c r="G77" s="22">
+        <v>106.5527</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>43831</v>
       </c>
@@ -1905,8 +2405,14 @@
       <c r="E78" s="14">
         <v>116.340759101602</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F78" s="21">
+        <v>598828.30000000005</v>
+      </c>
+      <c r="G78" s="22">
+        <v>108.6691</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>43922</v>
       </c>
@@ -1922,8 +2428,14 @@
       <c r="E79" s="14">
         <v>118.397887122821</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F79" s="21">
+        <v>554583.6</v>
+      </c>
+      <c r="G79" s="22">
+        <v>109.04900000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>44013</v>
       </c>
@@ -1939,8 +2451,14 @@
       <c r="E80" s="14">
         <v>119.17944207417</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F80" s="21">
+        <v>594916.30000000005</v>
+      </c>
+      <c r="G80" s="22">
+        <v>109.1846</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>44105</v>
       </c>
@@ -1956,8 +2474,14 @@
       <c r="E81" s="14">
         <v>122.56523297245</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F81" s="21">
+        <v>612691.30000000005</v>
+      </c>
+      <c r="G81" s="22">
+        <v>109.48309999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>44197</v>
       </c>
@@ -1973,8 +2497,14 @@
       <c r="E82" s="14">
         <v>124.254097916823</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F82" s="21">
+        <v>635701.1</v>
+      </c>
+      <c r="G82" s="22">
+        <v>111.708</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>44287</v>
       </c>
@@ -1990,8 +2520,14 @@
       <c r="E83" s="14">
         <v>124.43908937680099</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F83" s="21">
+        <v>652829.1</v>
+      </c>
+      <c r="G83" s="22">
+        <v>113.79730000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>44378</v>
       </c>
@@ -2007,8 +2543,14 @@
       <c r="E84" s="14">
         <v>125.906873191484</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F84" s="21">
+        <v>674135.4</v>
+      </c>
+      <c r="G84" s="22">
+        <v>114.93689999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>44470</v>
       </c>
@@ -2024,8 +2566,14 @@
       <c r="E85" s="14">
         <v>127.80160299542401</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F85" s="21">
+        <v>697934.8</v>
+      </c>
+      <c r="G85" s="22">
+        <v>118.003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>44562</v>
       </c>
@@ -2041,8 +2589,14 @@
       <c r="E86" s="14">
         <v>129.59988067281</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F86" s="21">
+        <v>731133.5</v>
+      </c>
+      <c r="G86" s="22">
+        <v>122.48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>44652</v>
       </c>
@@ -2058,8 +2612,14 @@
       <c r="E87" s="14">
         <v>136.18864304905901</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F87" s="21">
+        <v>759750.5</v>
+      </c>
+      <c r="G87" s="22">
+        <v>129.6703</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>44743</v>
       </c>
@@ -2075,8 +2635,14 @@
       <c r="E88" s="14">
         <v>141.102657877431</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F88" s="21">
+        <v>791479.1</v>
+      </c>
+      <c r="G88" s="22">
+        <v>133.76750000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>44835</v>
       </c>
@@ -2092,8 +2658,14 @@
       <c r="E89" s="14">
         <v>147.38535983267701</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F89" s="21">
+        <v>813267.2</v>
+      </c>
+      <c r="G89" s="22">
+        <v>138.67859999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>44927</v>
       </c>
@@ -2109,8 +2681,14 @@
       <c r="E90" s="14">
         <v>150.29476412206299</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F90" s="21">
+        <v>837619.5</v>
+      </c>
+      <c r="G90" s="22">
+        <v>144.29519999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>45017</v>
       </c>
@@ -2126,8 +2704,14 @@
       <c r="E91" s="14">
         <v>153.369561581249</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F91" s="21">
+        <v>849459.4</v>
+      </c>
+      <c r="G91" s="22">
+        <v>147.0085</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>45108</v>
       </c>
@@ -2143,8 +2727,14 @@
       <c r="E92" s="14">
         <v>151.84747137007301</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F92" s="21">
+        <v>856817.1</v>
+      </c>
+      <c r="G92" s="22">
+        <v>146.49299999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>45200</v>
       </c>
@@ -2160,8 +2750,14 @@
       <c r="E93" s="14">
         <v>154.34583014905601</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F93" s="21">
+        <v>868056.7</v>
+      </c>
+      <c r="G93" s="22">
+        <v>147.2799</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>45292</v>
       </c>
@@ -2177,8 +2773,14 @@
       <c r="E94" s="14">
         <v>155.55043293873899</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F94" s="21">
+        <v>881838.5</v>
+      </c>
+      <c r="G94" s="22">
+        <v>148.6908</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>45383</v>
       </c>
@@ -2194,8 +2796,14 @@
       <c r="E95" s="14">
         <v>156.40186902270099</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F95" s="21">
+        <v>899717.1</v>
+      </c>
+      <c r="G95" s="22">
+        <v>150.83439999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>45474</v>
       </c>
@@ -2211,8 +2819,14 @@
       <c r="E96" s="14">
         <v>159.00549014379101</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F96" s="21">
+        <v>915655.8</v>
+      </c>
+      <c r="G96" s="22">
+        <v>153.2764</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>45566</v>
       </c>
@@ -2228,8 +2842,14 @@
       <c r="E97" s="14">
         <v>160.41444462232499</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F97" s="21">
+        <v>936961.1</v>
+      </c>
+      <c r="G97" s="22">
+        <v>154.416</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>45658</v>
       </c>
@@ -2244,6 +2864,12 @@
       </c>
       <c r="E98" s="14">
         <v>160.646885330206</v>
+      </c>
+      <c r="F98" s="21">
+        <v>944654.7</v>
+      </c>
+      <c r="G98" s="22">
+        <v>156.64089999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>